<commit_message>
Playing around with models
</commit_message>
<xml_diff>
--- a/data/immoweb_real_estate_ml_ready_sample10_alberto.xlsx
+++ b/data/immoweb_real_estate_ml_ready_sample10_alberto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL11"/>
+  <dimension ref="A1:AN11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,135 +491,145 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>roomCount</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>hasAttic</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>hasBasement</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>hasDressingRoom</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>hasDiningRoom</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>buildingCondition</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>buildingConstructionYear</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>facedeCount</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>floorCount</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>hasLift</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>floodZoneType</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>heatingType</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>hasHeatPump</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>hasPhotovoltaicPanels</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>hasThermicPanels</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>kitchenType</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>hasLivingRoom</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>hasGarden</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>hasAirConditioning</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>hasArmoredDoor</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>hasVisiophone</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>hasOffice</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>toiletCount</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>hasSwimmingPool</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>hasFireplace</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>hasTerrace</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>epcScore</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>hasParking</t>
         </is>
@@ -673,66 +683,66 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>GOOD</t>
         </is>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>2004</v>
       </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
       <c r="S2" t="n">
         <v>1</v>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T2" t="n">
+        <v>7</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="inlineStr">
         <is>
           <t>NON_FLOOD_ZONE</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>GAS</t>
         </is>
       </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
       <c r="X2" t="n">
         <v>0</v>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="inlineStr">
         <is>
           <t>SEMI_EQUIPPED</t>
         </is>
       </c>
-      <c r="Z2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
       <c r="AB2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2" t="n">
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
         <v>0</v>
@@ -744,50 +754,56 @@
         <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="AK2" t="n">
+      <c r="AM2" t="n">
         <v>399000</v>
       </c>
-      <c r="AL2" t="b">
+      <c r="AN2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>20647642</v>
+        <v>20644816</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/house/for-sale/etterbeek/1040/20647642</t>
+          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20644816</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>HOUSE</t>
+          <t>APARTMENT</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>HOUSE</t>
+          <t>APARTMENT</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -803,66 +819,62 @@
         <v>1040</v>
       </c>
       <c r="K3" t="n">
-        <v>270</v>
+        <v>87</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>TO_BE_DONE_UP</t>
-        </is>
-      </c>
-      <c r="Q3" t="n">
-        <v>1910</v>
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>AS_NEW</t>
+        </is>
       </c>
       <c r="R3" t="n">
+        <v>1970</v>
+      </c>
+      <c r="S3" t="n">
         <v>2</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>NON_FLOOD_ZONE</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
+      <c r="T3" t="n">
+        <v>7</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr">
         <is>
           <t>FUELOIL</t>
         </is>
       </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
       <c r="X3" t="n">
         <v>0</v>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>INSTALLED</t>
-        </is>
+      <c r="Y3" t="n">
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>HYPER_EQUIPPED</t>
+        </is>
       </c>
       <c r="AB3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3" t="n">
         <v>0</v>
@@ -871,42 +883,48 @@
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
         <v>0</v>
       </c>
       <c r="AH3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
       </c>
       <c r="AK3" t="n">
-        <v>895000</v>
-      </c>
-      <c r="AL3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="AM3" t="n">
+        <v>465000</v>
+      </c>
+      <c r="AN3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>20644816</v>
+        <v>20659813</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20644816</t>
+          <t>https://www.immoweb.be/en/classified/apartment/for-sale/bruxelles/1040/20659813</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -923,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -932,14 +950,14 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Etterbeek</t>
+          <t>Bruxelles</t>
         </is>
       </c>
       <c r="J4" t="n">
         <v>1040</v>
       </c>
       <c r="K4" t="n">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -953,92 +971,102 @@
       <c r="O4" t="n">
         <v>0</v>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>AS_NEW</t>
         </is>
       </c>
-      <c r="Q4" t="n">
-        <v>1970</v>
-      </c>
       <c r="R4" t="n">
+        <v>2018</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>21</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>RECOGNIZED_FLOOD_ZONE</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>GAS</t>
+        </is>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>HYPER_EQUIPPED</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
         <v>2</v>
       </c>
-      <c r="S4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>FUELOIL</t>
-        </is>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>HYPER_EQUIPPED</t>
-        </is>
-      </c>
-      <c r="Z4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>0</v>
-      </c>
       <c r="AI4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>465000</v>
-      </c>
-      <c r="AL4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AM4" t="n">
+        <v>590000</v>
+      </c>
+      <c r="AN4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>20659813</v>
+        <v>20633249</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/apartment/for-sale/bruxelles/1040/20659813</t>
+          <t>https://www.immoweb.be/en/classified/flat-studio/for-sale/etterbeek/1040/20633249</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1048,14 +1076,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>APARTMENT</t>
+          <t>FLAT_STUDIO</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1064,14 +1092,14 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Bruxelles</t>
+          <t>Etterbeek</t>
         </is>
       </c>
       <c r="J5" t="n">
         <v>1040</v>
       </c>
       <c r="K5" t="n">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1085,94 +1113,102 @@
       <c r="O5" t="n">
         <v>0</v>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>AS_NEW</t>
         </is>
       </c>
-      <c r="Q5" t="n">
-        <v>2018</v>
-      </c>
-      <c r="R5" t="inlineStr"/>
+      <c r="R5" t="n">
+        <v>1906</v>
+      </c>
       <c r="S5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>RECOGNIZED_FLOOD_ZONE</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>NON_FLOOD_ZONE</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
         <is>
           <t>GAS</t>
         </is>
       </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0</v>
-      </c>
       <c r="X5" t="n">
         <v>0</v>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>HYPER_EQUIPPED</t>
-        </is>
+      <c r="Y5" t="n">
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>INSTALLED</t>
+        </is>
       </c>
       <c r="AB5" t="n">
         <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
         <v>0</v>
       </c>
       <c r="AF5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="n">
         <v>0</v>
       </c>
       <c r="AH5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
       </c>
       <c r="AK5" t="n">
-        <v>590000</v>
-      </c>
-      <c r="AL5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AM5" t="n">
+        <v>289000</v>
+      </c>
+      <c r="AN5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>20633249</v>
+        <v>20639359</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/flat-studio/for-sale/etterbeek/1040/20633249</t>
+          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20639359</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1182,11 +1218,11 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>FLAT_STUDIO</t>
+          <t>APARTMENT</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -1198,14 +1234,14 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Etterbeek</t>
+          <t>ETTERBEEK</t>
         </is>
       </c>
       <c r="J6" t="n">
         <v>1040</v>
       </c>
       <c r="K6" t="n">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -1214,57 +1250,53 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>AS_NEW</t>
-        </is>
-      </c>
-      <c r="Q6" t="n">
-        <v>1906</v>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>TO_BE_DONE_UP</t>
+        </is>
       </c>
       <c r="R6" t="n">
+        <v>1958</v>
+      </c>
+      <c r="S6" t="n">
         <v>2</v>
       </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>NON_FLOOD_ZONE</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
+      <c r="T6" t="n">
+        <v>6</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr">
         <is>
           <t>GAS</t>
         </is>
       </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0</v>
-      </c>
       <c r="X6" t="n">
         <v>0</v>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="inlineStr">
         <is>
           <t>INSTALLED</t>
         </is>
       </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
       <c r="AB6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6" t="n">
         <v>0</v>
@@ -1276,39 +1308,45 @@
         <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="n">
         <v>0</v>
       </c>
       <c r="AH6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" t="n">
         <v>0</v>
       </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
+      <c r="AJ6" t="n">
+        <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>289000</v>
-      </c>
-      <c r="AL6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AM6" t="n">
+        <v>375000</v>
+      </c>
+      <c r="AN6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>20639359</v>
+        <v>20634655</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20639359</t>
+          <t>https://www.immoweb.be/en/classified/duplex/for-sale/etterbeek/1040/20634655</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1318,7 +1356,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>APARTMENT</t>
+          <t>DUPLEX</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -1334,20 +1372,20 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ETTERBEEK</t>
+          <t>Etterbeek</t>
         </is>
       </c>
       <c r="J7" t="n">
         <v>1040</v>
       </c>
       <c r="K7" t="n">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -1355,92 +1393,102 @@
       <c r="O7" t="n">
         <v>0</v>
       </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>TO_BE_DONE_UP</t>
-        </is>
-      </c>
-      <c r="Q7" t="n">
-        <v>1958</v>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>AS_NEW</t>
+        </is>
       </c>
       <c r="R7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>5</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>NON_FLOOD_ZONE</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>GAS</t>
+        </is>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>HYPER_EQUIPPED</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH7" t="n">
         <v>2</v>
       </c>
-      <c r="S7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>GAS</t>
-        </is>
-      </c>
-      <c r="V7" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>INSTALLED</t>
-        </is>
-      </c>
-      <c r="Z7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>0</v>
-      </c>
       <c r="AI7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ7" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
       </c>
       <c r="AK7" t="n">
-        <v>375000</v>
-      </c>
-      <c r="AL7" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AM7" t="n">
+        <v>795000</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>20634658</v>
+        <v>20651309</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/duplex/for-sale/etterbeek/1040/20634658</t>
+          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20651309</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1450,14 +1498,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>DUPLEX</t>
+          <t>APARTMENT</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1473,110 +1521,112 @@
         <v>1040</v>
       </c>
       <c r="K8" t="n">
-        <v>220</v>
+        <v>93</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>JUST_RENOVATED</t>
-        </is>
-      </c>
-      <c r="Q8" t="n">
-        <v>2023</v>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>TO_BE_DONE_UP</t>
+        </is>
       </c>
       <c r="R8" t="n">
+        <v>1947</v>
+      </c>
+      <c r="S8" t="n">
         <v>2</v>
       </c>
-      <c r="S8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T8" t="inlineStr">
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>1</v>
+      </c>
+      <c r="V8" t="inlineStr">
         <is>
           <t>NON_FLOOD_ZONE</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>GAS</t>
-        </is>
-      </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0</v>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>FUELOIL</t>
+        </is>
       </c>
       <c r="X8" t="n">
         <v>0</v>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>HYPER_EQUIPPED</t>
-        </is>
+      <c r="Y8" t="n">
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8" t="n">
         <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="n">
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ8" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0</v>
       </c>
       <c r="AK8" t="n">
-        <v>950000</v>
-      </c>
-      <c r="AL8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="AM8" t="n">
+        <v>297000</v>
+      </c>
+      <c r="AN8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>20634657</v>
+        <v>20644613</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/duplex/for-sale/etterbeek/1040/20634657</t>
+          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20644613</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1586,14 +1636,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DUPLEX</t>
+          <t>APARTMENT</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1602,117 +1652,119 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Etterbeek</t>
+          <t>ETTERBEEK</t>
         </is>
       </c>
       <c r="J9" t="n">
         <v>1040</v>
       </c>
       <c r="K9" t="n">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>JUST_RENOVATED</t>
-        </is>
-      </c>
-      <c r="Q9" t="n">
-        <v>2023</v>
+        <v>1</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
       </c>
       <c r="R9" t="n">
+        <v>1932</v>
+      </c>
+      <c r="S9" t="n">
         <v>2</v>
       </c>
-      <c r="S9" t="n">
-        <v>1</v>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>NON_FLOOD_ZONE</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
+      <c r="T9" t="n">
+        <v>3</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr">
         <is>
           <t>GAS</t>
         </is>
       </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0</v>
-      </c>
       <c r="X9" t="n">
         <v>0</v>
       </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>HYPER_EQUIPPED</t>
-        </is>
+      <c r="Y9" t="n">
+        <v>0</v>
       </c>
       <c r="Z9" t="n">
         <v>0</v>
       </c>
-      <c r="AA9" t="n">
-        <v>0</v>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>INSTALLED</t>
+        </is>
       </c>
       <c r="AB9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9" t="n">
         <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AG9" t="n">
         <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ9" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0</v>
       </c>
       <c r="AK9" t="n">
-        <v>950000</v>
-      </c>
-      <c r="AL9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="AM9" t="n">
+        <v>435000</v>
+      </c>
+      <c r="AN9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>20634655</v>
+        <v>20577219</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/duplex/for-sale/etterbeek/1040/20634655</t>
+          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20577219</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1722,11 +1774,11 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>DUPLEX</t>
+          <t>APARTMENT</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -1745,7 +1797,7 @@
         <v>1040</v>
       </c>
       <c r="K10" t="n">
-        <v>187</v>
+        <v>119</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -1754,99 +1806,107 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>AS_NEW</t>
-        </is>
-      </c>
-      <c r="Q10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="R10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>TO_RENOVATE</t>
+        </is>
+      </c>
+      <c r="R10" t="n">
+        <v>1944</v>
+      </c>
       <c r="S10" t="n">
-        <v>1</v>
-      </c>
-      <c r="T10" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="T10" t="n">
+        <v>6</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1</v>
+      </c>
+      <c r="V10" t="inlineStr">
         <is>
           <t>NON_FLOOD_ZONE</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>GAS</t>
         </is>
       </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" t="n">
-        <v>0</v>
-      </c>
       <c r="X10" t="n">
         <v>0</v>
       </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>HYPER_EQUIPPED</t>
-        </is>
+      <c r="Y10" t="n">
+        <v>0</v>
       </c>
       <c r="Z10" t="n">
         <v>0</v>
       </c>
-      <c r="AA10" t="n">
-        <v>0</v>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>NOT_INSTALLED</t>
+        </is>
       </c>
       <c r="AB10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10" t="n">
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
         <v>1</v>
       </c>
       <c r="AF10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="n">
         <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0</v>
       </c>
       <c r="AK10" t="n">
-        <v>795000</v>
-      </c>
-      <c r="AL10" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AM10" t="n">
+        <v>370000</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>20651309</v>
+        <v>20653897</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.immoweb.be/en/classified/apartment/for-sale/etterbeek/1040/20651309</t>
+          <t>https://www.immoweb.be/en/classified/penthouse/for-sale/etterbeek/1040/20653897</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1856,11 +1916,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>APARTMENT</t>
+          <t>PENTHOUSE</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -1879,62 +1939,62 @@
         <v>1040</v>
       </c>
       <c r="K11" t="n">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>TO_BE_DONE_UP</t>
-        </is>
-      </c>
-      <c r="Q11" t="n">
-        <v>1947</v>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>AS_NEW</t>
+        </is>
       </c>
       <c r="R11" t="n">
+        <v>2024</v>
+      </c>
+      <c r="S11" t="n">
         <v>2</v>
       </c>
-      <c r="S11" t="n">
-        <v>1</v>
-      </c>
-      <c r="T11" t="inlineStr">
+      <c r="T11" t="n">
+        <v>4</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" t="inlineStr">
         <is>
           <t>NON_FLOOD_ZONE</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>FUELOIL</t>
-        </is>
-      </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>0</v>
-      </c>
+      <c r="W11" t="inlineStr"/>
       <c r="X11" t="n">
         <v>0</v>
       </c>
-      <c r="Y11" t="inlineStr"/>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
       <c r="Z11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>HYPER_EQUIPPED</t>
+        </is>
       </c>
       <c r="AB11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC11" t="n">
         <v>0</v>
@@ -1943,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11" t="n">
         <v>1</v>
@@ -1952,20 +2012,26 @@
         <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ11" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0</v>
       </c>
       <c r="AK11" t="n">
-        <v>297000</v>
-      </c>
-      <c r="AL11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AM11" t="n">
+        <v>735000</v>
+      </c>
+      <c r="AN11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>